<commit_message>
jan18,2017 added docs. gamay nalang!
</commit_message>
<xml_diff>
--- a/steps docs/Test Case/Test Case.xlsx
+++ b/steps docs/Test Case/Test Case.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -137,12 +137,226 @@
       <t>Functionality</t>
     </r>
   </si>
+  <si>
+    <t>Checking the Student (Freshmen/Transferee) gets a response when Admins have Apporved their Application Forms</t>
+  </si>
+  <si>
+    <t>Checking the Responsiveness between Student-Admin relationship when using the system</t>
+  </si>
+  <si>
+    <t>You must have a Student Account for STEPS
+You must Log in.
+Apply all Requirements and Wait for the Admin to Approve</t>
+  </si>
+  <si>
+    <t>1. Login STEPS (Student)
+2. Comply all the Requirements then wait
+3. Admin will Approve the requirements</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Student)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+username: rian
+Password: password
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Admin)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+username: sao
+Password: password</t>
+    </r>
+  </si>
+  <si>
+    <t>When the Admin has approved the student's requirements, it should be also Approved in Student's side</t>
+  </si>
+  <si>
+    <t>Requirements Approved</t>
+  </si>
+  <si>
+    <t>Checking if the student can't resume without a Student ID</t>
+  </si>
+  <si>
+    <t>Checking the security of the system</t>
+  </si>
+  <si>
+    <t>1. Login STEPS (Student)
+2. Comply all the Requirements then wait
+3. Not input a student ID</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Student)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+username: rian
+Password: password
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Admin)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+username: guidance
+Password: password</t>
+    </r>
+  </si>
+  <si>
+    <t>The System should only continue if the student has a student ID already</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>username:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> masteradmin
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Password: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">password
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Checking if the deletion of the Account would ask for your Confirmation or not</t>
+  </si>
+  <si>
+    <t>Checking the System if it's user-friendly</t>
+  </si>
+  <si>
+    <t>You must have a Student Account for STEPS
+You must Log in as a Master Admin.</t>
+  </si>
+  <si>
+    <t>1. Login STEPS (MasterAdmin)
+2. Delete an account.</t>
+  </si>
+  <si>
+    <t>Confirmation must be asked first before it could be deleted.</t>
+  </si>
+  <si>
+    <t>Account deleted when "Remove" button wa clicked</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,14 +368,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,6 +394,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -203,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -274,11 +496,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -297,8 +528,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -308,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -317,11 +546,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,15 +871,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:J23"/>
+  <dimension ref="C4:AX23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AQ5" sqref="AQ5:AX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" style="4" customWidth="1"/>
@@ -640,10 +887,37 @@
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.28515625" customWidth="1"/>
+    <col min="47" max="47" width="14.42578125" customWidth="1"/>
+    <col min="48" max="48" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:50" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,147 +942,363 @@
       <c r="J5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="12" t="s">
+      <c r="M5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU5" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AW5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="3:50" ht="243.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="14" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="3:10" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="13" t="s">
+      <c r="M6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="N6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="O6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="P6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="Q6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="R6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="S6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="W6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="X6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y6" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z6" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB6" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI6" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL6" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN6" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV6" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AW6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AX6" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="3:50" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="16" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="23"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="23"/>
+    </row>
+    <row r="8" spans="3:50" ht="210" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="6"/>
       <c r="G9" s="2"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="10"/>
+      <c r="I9" s="18"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="6"/>
       <c r="G10" s="2"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="10"/>
+      <c r="I10" s="18"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="6"/>
       <c r="G11" s="2"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="10"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="6"/>
       <c r="G12" s="2"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="10"/>
+      <c r="I12" s="18"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="6"/>
       <c r="G13" s="2"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="10"/>
+      <c r="I13" s="18"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="6"/>
       <c r="G14" s="2"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="10"/>
+      <c r="I14" s="18"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="6"/>
       <c r="G15" s="2"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="10"/>
+      <c r="I15" s="18"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="6"/>
       <c r="G16" s="2"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="18"/>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
@@ -818,7 +1308,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="2"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="10"/>
+      <c r="I17" s="18"/>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
@@ -828,7 +1318,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="2"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="10"/>
+      <c r="I18" s="18"/>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
@@ -838,7 +1328,7 @@
       <c r="F19" s="6"/>
       <c r="G19" s="2"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="10"/>
+      <c r="I19" s="18"/>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
@@ -848,7 +1338,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="2"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="10"/>
+      <c r="I20" s="18"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
@@ -858,7 +1348,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="2"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="10"/>
+      <c r="I21" s="18"/>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
@@ -868,7 +1358,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="2"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="10"/>
+      <c r="I22" s="18"/>
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -878,7 +1368,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="3"/>
       <c r="H23" s="9"/>
-      <c r="I23" s="11"/>
+      <c r="I23" s="19"/>
       <c r="J23" s="9"/>
     </row>
   </sheetData>

</xml_diff>